<commit_message>
minor template update for custom expression notation
</commit_message>
<xml_diff>
--- a/src/main/resources/org/jxls/demo/custom_expression_notation_template.xlsx
+++ b/src/main/resources/org/jxls/demo/custom_expression_notation_template.xlsx
@@ -86,9 +86,6 @@
     <t>Bonus</t>
   </si>
   <si>
-    <t>${employee.bonus}</t>
-  </si>
-  <si>
     <t>[[employee.name]]</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>Custom Expresssion Notation Demo</t>
+  </si>
+  <si>
+    <t>[[employee.bonus]]</t>
   </si>
 </sst>
 </file>
@@ -106,8 +106,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -186,8 +186,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -504,7 +504,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -527,16 +527,16 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="D4" s="6" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>